<commit_message>
feat: :sparkles: Finishing some details and generating some Images and Charts.
</commit_message>
<xml_diff>
--- a/research-in-acc-sciences/accountant-profile-in-startups/all_tables_article.xlsx
+++ b/research-in-acc-sciences/accountant-profile-in-startups/all_tables_article.xlsx
@@ -9,16 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tabela 1" sheetId="2" r:id="rId1"/>
     <sheet name="Tabela 2" sheetId="1" r:id="rId2"/>
-    <sheet name="techskills_final" sheetId="3" r:id="rId3"/>
-    <sheet name="idiomas" sheetId="5" r:id="rId4"/>
+    <sheet name="techskills_general" sheetId="6" r:id="rId3"/>
+    <sheet name="techskills_final_detailed" sheetId="3" r:id="rId4"/>
+    <sheet name="idiomas" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">techskills_final!$B$2:$F$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">techskills_final_detailed!$B$2:$F$25</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="68">
   <si>
     <t>Site de anúncio das vagas</t>
   </si>
@@ -201,13 +202,70 @@
   </si>
   <si>
     <t>fluente, inglês, chinês</t>
+  </si>
+  <si>
+    <t>Qtd.</t>
+  </si>
+  <si>
+    <t>% Qtd.</t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t>Sim</t>
+  </si>
+  <si>
+    <t>Pelo menos um conceito presente na 
+descrição da vaga</t>
+  </si>
+  <si>
+    <r>
+      <t>1 - Programação em Python (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Back-end</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>2 - Ciência de Dados</t>
+  </si>
+  <si>
+    <t>3 - Bancos de Dados</t>
+  </si>
+  <si>
+    <t>4 - Metodologias de Desenvolvimento</t>
+  </si>
+  <si>
+    <t>5 - Gestão de Projetos</t>
+  </si>
+  <si>
+    <t>6 - Ferramentas Diversas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -243,6 +301,14 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -380,18 +446,6 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -415,6 +469,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -699,7 +759,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -917,10 +977,322 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F11"/>
+  <dimension ref="B3:H19"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="1.85546875" style="12" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" style="12" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="12"/>
+    <col min="5" max="5" width="4.42578125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" style="12" customWidth="1"/>
+    <col min="7" max="8" width="9.140625" style="12"/>
+    <col min="9" max="9" width="1.85546875" style="12" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" s="32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="14">
+        <v>94</v>
+      </c>
+      <c r="D5" s="41">
+        <f>C5/$C$7</f>
+        <v>0.94</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" s="14">
+        <v>20</v>
+      </c>
+      <c r="H5" s="41">
+        <f>G5/$C$7</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="12">
+        <v>6</v>
+      </c>
+      <c r="D6" s="40">
+        <f>C6/$C$7</f>
+        <v>0.06</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" s="12">
+        <v>80</v>
+      </c>
+      <c r="H6" s="40">
+        <f>G6/$C$7</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="27">
+        <f>SUM(C5:C6)</f>
+        <v>100</v>
+      </c>
+      <c r="D7" s="42">
+        <f>C7/$C$7</f>
+        <v>1</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="27">
+        <f>SUM(G5:G6)</f>
+        <v>100</v>
+      </c>
+      <c r="H7" s="42">
+        <f>G7/$C$7</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" s="32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="14">
+        <v>73</v>
+      </c>
+      <c r="D11" s="41">
+        <f>C11/$C$7</f>
+        <v>0.73</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="14">
+        <v>100</v>
+      </c>
+      <c r="H11" s="41">
+        <f>G11/$C$7</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="12">
+        <v>27</v>
+      </c>
+      <c r="D12" s="40">
+        <f>C12/$C$7</f>
+        <v>0.27</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="12">
+        <v>0</v>
+      </c>
+      <c r="H12" s="40">
+        <f>G12/$C$7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="27">
+        <f>SUM(C11:C12)</f>
+        <v>100</v>
+      </c>
+      <c r="D13" s="42">
+        <f>C13/$C$7</f>
+        <v>1</v>
+      </c>
+      <c r="F13" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="27">
+        <f>SUM(G11:G12)</f>
+        <v>100</v>
+      </c>
+      <c r="H13" s="42">
+        <f>G13/$C$7</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="63" x14ac:dyDescent="0.25">
+      <c r="B16" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="H16" s="32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="14">
+        <v>75</v>
+      </c>
+      <c r="D17" s="41">
+        <f>C17/$C$7</f>
+        <v>0.75</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G17" s="14">
+        <v>100</v>
+      </c>
+      <c r="H17" s="41">
+        <f>G17/$C$7</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="12">
+        <v>25</v>
+      </c>
+      <c r="D18" s="40">
+        <f>C18/$C$7</f>
+        <v>0.25</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="G18" s="12">
+        <v>0</v>
+      </c>
+      <c r="H18" s="40">
+        <f>G18/$C$7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="27">
+        <f>SUM(C17:C18)</f>
+        <v>100</v>
+      </c>
+      <c r="D19" s="42">
+        <f>C19/$C$7</f>
+        <v>1</v>
+      </c>
+      <c r="F19" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="27">
+        <f>SUM(G17:G18)</f>
+        <v>100</v>
+      </c>
+      <c r="H19" s="42">
+        <f>G19/$C$7</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:F8"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -956,97 +1328,79 @@
         <v>12</v>
       </c>
       <c r="D3" s="29">
-        <f>C3/$C$10</f>
+        <f>C3/$C$7</f>
         <v>0.52173913043478259</v>
       </c>
       <c r="E3" s="26" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="32"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="35"/>
-    </row>
-    <row r="5" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="20">
+        <v>6</v>
+      </c>
+      <c r="D4" s="30">
+        <f>C4/$C$7</f>
+        <v>0.2608695652173913</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="20">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D5" s="30">
-        <f t="shared" ref="D5:D9" si="0">C5/$C$10</f>
-        <v>0.2608695652173913</v>
+        <f>C5/$C$7</f>
+        <v>0.17391304347826086</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="17"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="18"/>
-    </row>
-    <row r="7" spans="2:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="20">
-        <v>4</v>
-      </c>
-      <c r="D7" s="30">
-        <f t="shared" si="0"/>
-        <v>0.17391304347826086</v>
-      </c>
-      <c r="E7" s="18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="17"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="18"/>
-    </row>
-    <row r="9" spans="2:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="17" t="s">
+    <row r="6" spans="2:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="20">
-        <v>1</v>
-      </c>
-      <c r="D9" s="30">
-        <f t="shared" si="0"/>
+      <c r="C6" s="20">
+        <v>1</v>
+      </c>
+      <c r="D6" s="30">
+        <f>C6/$C$7</f>
         <v>4.3478260869565216E-2</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E6" s="18" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="27" t="s">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="28">
-        <f>SUM(C3:C9)</f>
+      <c r="C7" s="28">
+        <f>SUM(C3:C6)</f>
         <v>23</v>
       </c>
-      <c r="D10" s="31">
-        <f>SUM(D3:D9)</f>
+      <c r="D7" s="31">
+        <f>SUM(D3:D6)</f>
         <v>0.99999999999999989</v>
       </c>
-      <c r="E10" s="14"/>
-    </row>
-    <row r="11" spans="2:5" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="E7" s="14"/>
+    </row>
+    <row r="8" spans="2:5" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -1059,14 +1413,14 @@
     <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="173.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="33" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1074,10 +1428,10 @@
       <c r="A2" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="38">
+      <c r="B2" s="34">
         <v>36</v>
       </c>
-      <c r="C2" s="39">
+      <c r="C2" s="35">
         <v>0.36</v>
       </c>
     </row>
@@ -1085,107 +1439,107 @@
       <c r="A3" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="40">
+      <c r="B3" s="36">
         <v>64</v>
       </c>
-      <c r="C3" s="41">
+      <c r="C3" s="37">
         <v>0.64000000000000012</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="43">
+      <c r="B4" s="39">
         <v>31</v>
       </c>
-      <c r="C4" s="41">
+      <c r="C4" s="37">
         <v>0.31</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="43">
+      <c r="B5" s="39">
         <v>14</v>
       </c>
-      <c r="C5" s="41">
+      <c r="C5" s="37">
         <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="43">
+      <c r="B6" s="39">
         <v>7</v>
       </c>
-      <c r="C6" s="41">
+      <c r="C6" s="37">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="43">
+      <c r="B7" s="39">
         <v>5</v>
       </c>
-      <c r="C7" s="41">
+      <c r="C7" s="37">
         <v>0.05</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="43">
+      <c r="B8" s="39">
         <v>4</v>
       </c>
-      <c r="C8" s="41">
+      <c r="C8" s="37">
         <v>0.04</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="43">
-        <v>1</v>
-      </c>
-      <c r="C9" s="41">
+      <c r="B9" s="39">
+        <v>1</v>
+      </c>
+      <c r="C9" s="37">
         <v>0.01</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="43">
-        <v>1</v>
-      </c>
-      <c r="C10" s="41">
+      <c r="B10" s="39">
+        <v>1</v>
+      </c>
+      <c r="C10" s="37">
         <v>0.01</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="43">
-        <v>1</v>
-      </c>
-      <c r="C11" s="41">
+      <c r="B11" s="39">
+        <v>1</v>
+      </c>
+      <c r="C11" s="37">
         <v>0.01</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
-      <c r="B12" s="38">
+      <c r="B12" s="34">
         <v>100</v>
       </c>
-      <c r="C12" s="39">
+      <c r="C12" s="35">
         <v>1</v>
       </c>
     </row>

</xml_diff>